<commit_message>
Add tests for permission update during migration.
</commit_message>
<xml_diff>
--- a/opengever/bundle/tests/assets/os_migration/os_test_create.xlsx
+++ b/opengever/bundle/tests/assets/os_migration/os_test_create.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Work/development/opengever.core/opengever/bundle/tests/assets/os_migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F56A050-C730-AA41-899E-454C29FFFAD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40EB105-DE37-594D-9581-EA90A06EA040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="5460" windowWidth="25920" windowHeight="10340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="100">
   <si>
     <t>reference_number</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>New description</t>
+  </si>
+  <si>
+    <t>group1, group2</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2, group3</t>
   </si>
 </sst>
 </file>
@@ -1577,9 +1586,9 @@
   <sheetPr codeName="Blatt1"/>
   <dimension ref="A1:Z512"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1967,11 +1976,17 @@
       </c>
       <c r="R7" s="62"/>
       <c r="S7" s="63"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
+      <c r="T7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="V7" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
     </row>
@@ -2105,11 +2120,21 @@
       <c r="Q11" s="11"/>
       <c r="R11" s="12"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
+      <c r="T11" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="V11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="W11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X11" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
@@ -13871,7 +13896,7 @@
           <x14:formula1>
             <xm:f>Wertebereich!$O$2:$O$4</xm:f>
           </x14:formula1>
-          <xm:sqref>T11:T1048576</xm:sqref>
+          <xm:sqref>T11:T1048576 T7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -13911,7 +13936,7 @@
   <sheetPr codeName="Blatt2"/>
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -14084,27 +14109,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <oc_termin_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
-    <oc_traktandum_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
-    <oc_termin_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
-    <oc_document_is_common xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
-    <oc_traktandum_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100440900994F0F214B9EC76DEC64CCCEC3" ma:contentTypeVersion="" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="3c93ed4d6daf505d37aacf3e1bef2534">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="96CA5592-7E49-4C69-936A-77E0F19F316B" xmlns:ns3="82675a1d-2274-46ff-95b6-7e628f04e7b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c3cc4f1e90dff483e4da45e10a5d6cb" ns2:_="" ns3:_="">
     <xsd:import namespace="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
@@ -14295,10 +14299,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <oc_termin_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
+    <oc_traktandum_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
+    <oc_termin_lookup xmlns="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
+    <oc_document_is_common xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
+    <oc_traktandum_lookup_helper xmlns="82675a1d-2274-46ff-95b6-7e628f04e7b8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B73656-B986-42B5-A6F0-2CB7C4F8F507}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37806679-E8E8-4A87-9E25-D47F01162BB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
+    <ds:schemaRef ds:uri="82675a1d-2274-46ff-95b6-7e628f04e7b8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14315,20 +14351,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37806679-E8E8-4A87-9E25-D47F01162BB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B73656-B986-42B5-A6F0-2CB7C4F8F507}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="96CA5592-7E49-4C69-936A-77E0F19F316B"/>
-    <ds:schemaRef ds:uri="82675a1d-2274-46ff-95b6-7e628f04e7b8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>